<commit_message>
[IMP] Adjust Payable Detail Report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_payable_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_payable_detail.xlsx
@@ -20,9 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
-  <si>
-    <t xml:space="preserve">รายงานรายละเอียดเจ้าหนี้รายตัว</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+  <si>
+    <t xml:space="preserve">Real Start Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payable Detail Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real End Date</t>
   </si>
   <si>
     <t xml:space="preserve">Account Code</t>
@@ -37,22 +43,25 @@
     <t xml:space="preserve">Fiscal Year To</t>
   </si>
   <si>
+    <t xml:space="preserve">Filter by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period Length (days)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Period From</t>
   </si>
   <si>
     <t xml:space="preserve">Period To</t>
   </si>
   <si>
-    <t xml:space="preserve">Document Posting Date From</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document Posting Date To</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document Date From</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document Date To</t>
+    <t xml:space="preserve">Date From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As of Date</t>
   </si>
   <si>
     <t xml:space="preserve">Document Number</t>
@@ -89,6 +98,12 @@
   </si>
   <si>
     <t xml:space="preserve">Due Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overdue (Days)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overdue Length</t>
   </si>
   <si>
     <t xml:space="preserve">Source Document Ref.</t>
@@ -146,8 +161,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
+    <numFmt numFmtId="167" formatCode="#,###.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -179,7 +197,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,8 +206,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADD58A"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFCCCCFF"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -233,28 +263,68 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -271,6 +341,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFADD58A"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -279,10 +409,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA13"/>
+  <dimension ref="A1:AMJ15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5:C8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -290,192 +420,328 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="26.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="23.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="21.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="21.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="24.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="22.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="25.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="25.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="21.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="20.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="23.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="23.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="25.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="19.17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="28" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="22.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="26.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="21.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="6" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="6" width="24.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="22.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="25.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="25.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="6" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="22.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="6" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="32" min="30" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="24.03"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="35" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A1" s="7"/>
+      <c r="F1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="AG1" s="8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="AH1" s="9"/>
+    </row>
+    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="AG2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="AH2" s="9"/>
+      <c r="AME2" s="0"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3" t="s">
+      <c r="B3" s="11"/>
+      <c r="AME3" s="0"/>
+      <c r="AMF3" s="0"/>
+      <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
+    </row>
+    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="B4" s="11"/>
+      <c r="AME4" s="0"/>
+      <c r="AMF4" s="0"/>
+      <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="D5" s="11"/>
+      <c r="AG5" s="12"/>
+      <c r="AH5" s="13"/>
+      <c r="AME5" s="0"/>
+      <c r="AMF5" s="0"/>
+      <c r="AMG5" s="0"/>
+      <c r="AMH5" s="0"/>
+      <c r="AMI5" s="0"/>
+      <c r="AMJ5" s="0"/>
+    </row>
+    <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="7"/>
+      <c r="AG6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="AH6" s="9"/>
+      <c r="AME6" s="0"/>
+      <c r="AMF6" s="0"/>
+      <c r="AMG6" s="0"/>
+      <c r="AMH6" s="0"/>
+      <c r="AMI6" s="0"/>
+      <c r="AMJ6" s="0"/>
+    </row>
+    <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="D7" s="11"/>
+      <c r="AH7" s="9"/>
+      <c r="AME7" s="0"/>
+      <c r="AMF7" s="0"/>
+      <c r="AMG7" s="0"/>
+      <c r="AMH7" s="0"/>
+      <c r="AMI7" s="0"/>
+      <c r="AMJ7" s="0"/>
+    </row>
+    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="D8" s="14"/>
+      <c r="AH8" s="9"/>
+      <c r="AME8" s="0"/>
+      <c r="AMF8" s="0"/>
+      <c r="AMG8" s="0"/>
+      <c r="AMH8" s="0"/>
+      <c r="AMI8" s="0"/>
+      <c r="AMJ8" s="0"/>
+    </row>
+    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="13" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="7"/>
+      <c r="AH9" s="9"/>
+      <c r="AME9" s="0"/>
+      <c r="AMF9" s="0"/>
+      <c r="AMG9" s="0"/>
+      <c r="AMH9" s="0"/>
+      <c r="AMI9" s="0"/>
+      <c r="AMJ9" s="0"/>
+    </row>
+    <row r="10" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="7"/>
+      <c r="AH10" s="13"/>
+      <c r="AME10" s="0"/>
+      <c r="AMF10" s="0"/>
+      <c r="AMG10" s="0"/>
+      <c r="AMH10" s="0"/>
+      <c r="AMI10" s="0"/>
+      <c r="AMJ10" s="0"/>
+    </row>
+    <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B11" s="11"/>
+      <c r="AME11" s="0"/>
+      <c r="AMF11" s="0"/>
+      <c r="AMG11" s="0"/>
+      <c r="AMH11" s="0"/>
+      <c r="AMI11" s="0"/>
+      <c r="AMJ11" s="0"/>
+    </row>
+    <row r="12" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="B12" s="11"/>
+      <c r="AME12" s="0"/>
+      <c r="AMF12" s="0"/>
+      <c r="AMG12" s="0"/>
+      <c r="AMH12" s="0"/>
+      <c r="AMI12" s="0"/>
+      <c r="AMJ12" s="0"/>
+    </row>
+    <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="B13" s="11"/>
+      <c r="AME13" s="0"/>
+      <c r="AMF13" s="0"/>
+      <c r="AMG13" s="0"/>
+      <c r="AMH13" s="0"/>
+      <c r="AMI13" s="0"/>
+      <c r="AMJ13" s="0"/>
+    </row>
+    <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AME14" s="0"/>
+      <c r="AMF14" s="0"/>
+      <c r="AMG14" s="0"/>
+      <c r="AMH14" s="0"/>
+      <c r="AMI14" s="0"/>
+      <c r="AMJ14" s="0"/>
+    </row>
+    <row r="15" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="5" t="s">
+      <c r="B15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="C15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="D15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="E15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="G15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="H15" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="I15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="J15" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="K15" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="L15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="P13" s="5" t="s">
+      <c r="M15" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Q13" s="5" t="s">
+      <c r="N15" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="R13" s="5" t="s">
+      <c r="O15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="S13" s="5" t="s">
+      <c r="P15" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="T13" s="5" t="s">
+      <c r="Q15" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="U13" s="5" t="s">
+      <c r="R15" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="V13" s="5" t="s">
+      <c r="S15" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="W13" s="5" t="s">
+      <c r="T15" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="X13" s="5" t="s">
+      <c r="U15" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="Y13" s="5" t="s">
+      <c r="V15" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="Z13" s="5" t="s">
+      <c r="W15" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AA13" s="5" t="s">
+      <c r="X15" s="15" t="s">
         <v>39</v>
       </c>
+      <c r="Y15" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA15" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AME15" s="0"/>
+      <c r="AMF15" s="0"/>
+      <c r="AMG15" s="0"/>
+      <c r="AMH15" s="0"/>
+      <c r="AMI15" s="0"/>
+      <c r="AMJ15" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
[FIX] #2984 report payable detail
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_payable_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_payable_detail.xlsx
@@ -263,7 +263,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -313,6 +313,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -634,7 +638,7 @@
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
-    <row r="15" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
@@ -665,10 +669,10 @@
       <c r="J15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="13" t="s">
         <v>27</v>
       </c>
       <c r="M15" s="12" t="s">

</xml_diff>

<commit_message>
[IMP] Adjust payable and receivable detail report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_payable_detail.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_payable_detail.xlsx
@@ -326,12 +326,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -441,7 +441,9 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="32" min="30" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="25.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="24.03"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="35" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="50" min="35" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="52" min="51" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="53" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>

</xml_diff>